<commit_message>
complete covid flow tested xml to es, es to xlsx, xlsx template
</commit_message>
<xml_diff>
--- a/resources/data_example/standaardverslag_covid.xlsx
+++ b/resources/data_example/standaardverslag_covid.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\nlp-datau\resources\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\nlp-datau\resources\data_example\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,9 +26,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>source</t>
-  </si>
-  <si>
     <t>Blanco CT Thorax 
 COVID 19 Standaardverslag 
 1. Klachten {    }
@@ -44,6 +41,9 @@
  {   }
 Nevenbevindingen: { Dit is een hele vreemde bevinding   }
 DISCLAIMER: De interobserver variatie bij CORADS ....</t>
+  </si>
+  <si>
+    <t>text</t>
   </si>
 </sst>
 </file>
@@ -366,20 +366,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="409.5" x14ac:dyDescent="0.75">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.75">

</xml_diff>